<commit_message>
docs: create and link to iadd-0x01
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="293">
   <si>
     <t>TYPE</t>
   </si>
@@ -131,10 +131,10 @@
     <t>lconst</t>
   </si>
   <si>
-    <t>将常量池中以arg1为偏移量的number常量作为对象添加到堆并将堆偏移量push到栈</t>
-  </si>
-  <si>
-    <t>stack.push2( cp_pool[arg1] );</t>
+    <t>u8</t>
+  </si>
+  <si>
+    <t>stack.push2( arg1 );</t>
   </si>
   <si>
     <t>08</t>
@@ -155,7 +155,7 @@
     <t>ladd</t>
   </si>
   <si>
-    <t>将栈顶两个long相加（每个八字节）并将结果push到栈顶</t>
+    <t>将栈顶两个long相加（每个8字节）并将结果push到栈顶</t>
   </si>
   <si>
     <t>stack.push2( (stack.pop2()) + (stack.pop2() );</t>
@@ -164,6 +164,18 @@
     <t>0A</t>
   </si>
   <si>
+    <t>fadd</t>
+  </si>
+  <si>
+    <t>将栈顶两个float相加（每个8字节）并将结果push到栈顶</t>
+  </si>
+  <si>
+    <t>stack.pushf( (stack.popf()) + (stack.popf() );</t>
+  </si>
+  <si>
+    <t>0B</t>
+  </si>
+  <si>
     <t>isub</t>
   </si>
   <si>
@@ -173,7 +185,7 @@
     <t>top = stack.pop(); top_m1 = stack.pop(); stack.push(a-b);</t>
   </si>
   <si>
-    <t>0B</t>
+    <t>0C</t>
   </si>
   <si>
     <t>lsub</t>
@@ -185,7 +197,16 @@
     <t>top = stack.pop2(); top_m1 = stack.pop2(); stack.push2( top - top_m1 );</t>
   </si>
   <si>
-    <t>0C</t>
+    <t>0D</t>
+  </si>
+  <si>
+    <t>isub的float版本</t>
+  </si>
+  <si>
+    <t>top = stack.popf(); top_m1 = stack.popf(); stack.pushf( top - top_m1 );</t>
+  </si>
+  <si>
+    <t>0E</t>
   </si>
   <si>
     <t>imul</t>
@@ -197,7 +218,7 @@
     <t>stack.push( (stack.pop()) * (stack.pop()) );</t>
   </si>
   <si>
-    <t>0D</t>
+    <t>0F</t>
   </si>
   <si>
     <t>lmul</t>
@@ -209,7 +230,19 @@
     <t>stack.push2( stack.pop2() * stack.pop2() );</t>
   </si>
   <si>
-    <t>0E</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>fmul</t>
+  </si>
+  <si>
+    <t>imul的float版本</t>
+  </si>
+  <si>
+    <t>stack.pushf( stack.popf() * stack.popf() );</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>idiv</t>
@@ -221,7 +254,7 @@
     <t>obj = stack.pop(); dvder = stack.pop(); stack.push(obj / dvder);</t>
   </si>
   <si>
-    <t>0F</t>
+    <t>12</t>
   </si>
   <si>
     <t>ldiv</t>
@@ -233,7 +266,19 @@
     <t>obj = stack.pop2(); dvder = stack.pop2(); stack.push2(obj / dvder);</t>
   </si>
   <si>
-    <t>10</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>fdiv</t>
+  </si>
+  <si>
+    <t>idiv的float版本</t>
+  </si>
+  <si>
+    <t>obj = stack.popf(); dvder = stack.popf(); stack.pushf(obj / dvder);</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
   <si>
     <t>irem</t>
@@ -245,7 +290,7 @@
     <t>obj = stack.pop(); dvder = stack.pop(); stack.push(obj % dvder);</t>
   </si>
   <si>
-    <t>11</t>
+    <t>15</t>
   </si>
   <si>
     <t>lrem</t>
@@ -257,7 +302,19 @@
     <t>obj = stack.pop2(); dvder = stack.pop2(); stack.push2(obj % dvder);</t>
   </si>
   <si>
-    <t>12</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>frem</t>
+  </si>
+  <si>
+    <t>irem的float版本</t>
+  </si>
+  <si>
+    <t>obj = stack.popf(); dvder = stack.popf(); stack.pushf(obj % dvder);</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
   <si>
     <t>ineg</t>
@@ -269,19 +326,31 @@
     <t>stack.push( -(stack.pop()) );</t>
   </si>
   <si>
-    <t>13</t>
+    <t>18</t>
   </si>
   <si>
     <t>lneg</t>
   </si>
   <si>
-    <t>ineg的双字版本</t>
+    <t>ineg的long版本</t>
   </si>
   <si>
     <t>stack.push2( -stack.pop2() );</t>
   </si>
   <si>
-    <t>14</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t>fneg</t>
+  </si>
+  <si>
+    <t>ineg的float版本</t>
+  </si>
+  <si>
+    <t>stack.pushf( -stack.popf() );</t>
+  </si>
+  <si>
+    <t>1A</t>
   </si>
   <si>
     <t>iexp</t>
@@ -293,19 +362,31 @@
     <t>base = stack.pop(); exp = stack.pop(); stack.push(base ^ exp);</t>
   </si>
   <si>
-    <t>15</t>
+    <t>1B</t>
   </si>
   <si>
     <t>lexp</t>
   </si>
   <si>
-    <t>iexp的双字版本</t>
+    <t>iexp的long版本</t>
   </si>
   <si>
     <t>base=stack.pop2();exp=stack.pop2();stack.push2(base ^ exp);</t>
   </si>
   <si>
-    <t>16</t>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>fexp</t>
+  </si>
+  <si>
+    <t>iexp的float版本</t>
+  </si>
+  <si>
+    <t>base=stack.popf();exp=stack.popf();stack.pushf(base ^ exp);</t>
+  </si>
+  <si>
+    <t>1D</t>
   </si>
   <si>
     <t>ishl</t>
@@ -317,7 +398,7 @@
     <t>base = stack.pop(); stack.push( base &gt;&gt; (stack.pop()) );</t>
   </si>
   <si>
-    <t>17</t>
+    <t>1E</t>
   </si>
   <si>
     <t>lshl</t>
@@ -329,7 +410,7 @@
     <t>base = stack.pop2(); stack.push2( base &gt;&gt; (stack.pop2()) );</t>
   </si>
   <si>
-    <t>18</t>
+    <t>1F</t>
   </si>
   <si>
     <t>ishr</t>
@@ -341,7 +422,7 @@
     <t>base = stack.pop(); stack.push( base &lt;&lt; (stack.pop()) );</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>lshr</t>
@@ -353,7 +434,7 @@
     <t>base = stack.pop2(); stack.push2( base &lt;&lt; (stack.pop2()) );</t>
   </si>
   <si>
-    <t>1A</t>
+    <t>21</t>
   </si>
   <si>
     <t>ixnd</t>
@@ -365,7 +446,7 @@
     <t>stack.push( stack.pop() &amp; stack.pop() );</t>
   </si>
   <si>
-    <t>1B</t>
+    <t>22</t>
   </si>
   <si>
     <t>lxnd</t>
@@ -377,7 +458,7 @@
     <t>stack.push( stack.pop2() &amp; stack.pop2() );</t>
   </si>
   <si>
-    <t>1C</t>
+    <t>23</t>
   </si>
   <si>
     <t>ixor</t>
@@ -389,7 +470,7 @@
     <t>stack.push( stack.pop() | stack.pop() );</t>
   </si>
   <si>
-    <t>1D</t>
+    <t>24</t>
   </si>
   <si>
     <t>lxor</t>
@@ -401,7 +482,7 @@
     <t>stack.push( stack.pop2() | stack.pop2() );</t>
   </si>
   <si>
-    <t>1E</t>
+    <t>25</t>
   </si>
   <si>
     <t>bnd</t>
@@ -413,7 +494,7 @@
     <t>特殊实现：栈一个格4byte，前两byte存两个bool进行运算，第三个格为00时与运算，为01时或运算，第四个废弃</t>
   </si>
   <si>
-    <t>1F</t>
+    <t>26</t>
   </si>
   <si>
     <t>bor</t>
@@ -422,7 +503,7 @@
     <t>将栈顶两数按bool或</t>
   </si>
   <si>
-    <t>20</t>
+    <t>27</t>
   </si>
   <si>
     <t>icmp</t>
@@ -434,19 +515,31 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); stack.push( (a1 == a2) ? 0 :  ( (a1&lt;a2) ? -1 : 1 ) );</t>
   </si>
   <si>
-    <t>21</t>
+    <t>28</t>
   </si>
   <si>
     <t>lcmp</t>
   </si>
   <si>
-    <t>icmp的双字版本</t>
-  </si>
-  <si>
-    <t>a1 = stack.pop2(); a2 = stack.pop2(); stack.push( (a1 == a2) ? 0 :  ( (a1&lt;a2) ? -1 : 1 ) );</t>
-  </si>
-  <si>
-    <t>22</t>
+    <t>icmp的long版本</t>
+  </si>
+  <si>
+    <t>a1 = stack.pop2(); a2 = stack.pop2(); stack.push2( (a1 == a2) ? 0 :  ( (a1&lt;a2) ? -1 : 1 ) );</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>fcmp</t>
+  </si>
+  <si>
+    <t>icmp的float版本</t>
+  </si>
+  <si>
+    <t>a1 = stack.popf(); a2 = stack.popf(); stack.pushf( (a1 == a2) ? 0 :  ( (a1&lt;a2) ? -1 : 1 ) );</t>
+  </si>
+  <si>
+    <t>2A</t>
   </si>
   <si>
     <t>goto</t>
@@ -458,7 +551,7 @@
     <t>jmp( startadr + arg1 );</t>
   </si>
   <si>
-    <t>23</t>
+    <t>2B</t>
   </si>
   <si>
     <t>goto_w</t>
@@ -470,7 +563,7 @@
     <t>ljmp( startadr + arg1 );</t>
   </si>
   <si>
-    <t>24</t>
+    <t>2C</t>
   </si>
   <si>
     <t>goto_o</t>
@@ -485,7 +578,7 @@
     <t>jmp( current + arg1 );</t>
   </si>
   <si>
-    <t>25</t>
+    <t>2D</t>
   </si>
   <si>
     <t>ifeq</t>
@@ -497,7 +590,7 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); if(a1==a2){ jmp(current+arg1); }</t>
   </si>
   <si>
-    <t>26</t>
+    <t>2E</t>
   </si>
   <si>
     <t>ifeq_w</t>
@@ -509,7 +602,7 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); if(a1==a2){ ljmp(current+arg1); }</t>
   </si>
   <si>
-    <t>27</t>
+    <t>2F</t>
   </si>
   <si>
     <t>ifne</t>
@@ -518,7 +611,7 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); if(a1!=a2){ jmp(current+arg1); }</t>
   </si>
   <si>
-    <t>28</t>
+    <t>30</t>
   </si>
   <si>
     <t>ifne_w</t>
@@ -530,7 +623,7 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); if(a1!=a2){ ljmp(current+arg1); }</t>
   </si>
   <si>
-    <t>29</t>
+    <t>31</t>
   </si>
   <si>
     <t>iflt</t>
@@ -542,7 +635,7 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); if(a1&lt;a2){ jmp(current+arg1); }</t>
   </si>
   <si>
-    <t>2A</t>
+    <t>32</t>
   </si>
   <si>
     <t>ifle</t>
@@ -554,7 +647,7 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); if(a1&lt;=a2){ jmp(current+arg1); }</t>
   </si>
   <si>
-    <t>2B</t>
+    <t>33</t>
   </si>
   <si>
     <t>ifgt</t>
@@ -566,7 +659,7 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); if(a1&gt;a2){ jmp(current+arg1); }</t>
   </si>
   <si>
-    <t>2C</t>
+    <t>34</t>
   </si>
   <si>
     <t>ifge</t>
@@ -578,7 +671,7 @@
     <t>a1 = stack.pop(); a2 = stack.pop(); if(a1&gt;=a2){ jmp(current+arg1); }</t>
   </si>
   <si>
-    <t>2D</t>
+    <t>35</t>
   </si>
   <si>
     <t>ifnull</t>
@@ -590,7 +683,7 @@
     <t>base = stack.pop(); stack.push( base == 1 | base == null );</t>
   </si>
   <si>
-    <t>2E</t>
+    <t>36</t>
   </si>
   <si>
     <t>lifnull</t>
@@ -602,7 +695,7 @@
     <t>base = heap[stack.pop()]; stack.push( base==1 | base==null );</t>
   </si>
   <si>
-    <t>2F</t>
+    <t>37</t>
   </si>
   <si>
     <t>ret</t>
@@ -614,16 +707,22 @@
     <t>jmp(ret_address);</t>
   </si>
   <si>
-    <t>30</t>
+    <t>38</t>
   </si>
   <si>
     <t>tswitch</t>
   </si>
   <si>
-    <t>tableswitch，</t>
-  </si>
-  <si>
-    <t>31</t>
+    <t>arg1：u2
+arg2：u2
+arg3：u2
+arg4：u1</t>
+  </si>
+  <si>
+    <t>将arg1作为最低case，arg2作为最高case，arg3为第一个匹配项的值，arg4作为公差</t>
+  </si>
+  <si>
+    <t>39</t>
   </si>
   <si>
     <t>lswitch</t>
@@ -632,16 +731,16 @@
     <t>lookupswitch</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>3D</t>
   </si>
   <si>
     <t>pconst</t>
@@ -653,7 +752,7 @@
     <t>stack.push( cp_pool[arg1] );</t>
   </si>
   <si>
-    <t>36</t>
+    <t>3E</t>
   </si>
   <si>
     <t>sconst</t>
@@ -665,7 +764,7 @@
     <t>localvar[arg2] = cp_pool[arg1];</t>
   </si>
   <si>
-    <t>37</t>
+    <t>3F</t>
   </si>
   <si>
     <t>push</t>
@@ -677,7 +776,7 @@
     <t xml:space="preserve">stack.push( local[var2] ); </t>
   </si>
   <si>
-    <t>38</t>
+    <t>40</t>
   </si>
   <si>
     <t>pop</t>
@@ -689,7 +788,7 @@
     <t>localvar[arg1] = stack.pop();</t>
   </si>
   <si>
-    <t>39</t>
+    <t>41</t>
   </si>
   <si>
     <t>pop2</t>
@@ -701,9 +800,6 @@
     <t>localvar[arg1] = stack.pop2();</t>
   </si>
   <si>
-    <t>3A</t>
-  </si>
-  <si>
     <t>dup</t>
   </si>
   <si>
@@ -713,9 +809,6 @@
     <t>t1 = stack.pop(); t2 = stack.pop(); stack.push(t1); stack.push(t2);</t>
   </si>
   <si>
-    <t>3B</t>
-  </si>
-  <si>
     <t>new</t>
   </si>
   <si>
@@ -725,9 +818,6 @@
     <t>ret_address = current;  stack.push( call(cp_pool[arg1], "_init", stack );</t>
   </si>
   <si>
-    <t>3C</t>
-  </si>
-  <si>
     <t>newarr</t>
   </si>
   <si>
@@ -737,18 +827,12 @@
     <t>ret_address = current;  stack.push( call(cp_pool + "$array", "_init", stack );</t>
   </si>
   <si>
-    <t>3D</t>
-  </si>
-  <si>
     <t>call</t>
   </si>
   <si>
     <t>ret_address = current;  stack.push( call(cp_pool[arg1], cp_pool[arg2], stack );</t>
   </si>
   <si>
-    <t>3E</t>
-  </si>
-  <si>
     <t>getField</t>
   </si>
   <si>
@@ -758,9 +842,6 @@
     <t>obj = stack.pop(); stack.push( obj.fields[arg1] );</t>
   </si>
   <si>
-    <t>3F</t>
-  </si>
-  <si>
     <t>putField</t>
   </si>
   <si>
@@ -770,9 +851,6 @@
     <t>obj = stack.pop(); obj.fields[arg1] = stack.pop();</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>sp_enter</t>
   </si>
   <si>
@@ -782,9 +860,6 @@
     <t xml:space="preserve">-  </t>
   </si>
   <si>
-    <t>41</t>
-  </si>
-  <si>
     <t>sp_quit</t>
   </si>
   <si>
@@ -792,6 +867,39 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>一些声明</t>
+  </si>
+  <si>
+    <t>伪代码栏中，含有stack,call等变量、函数，这是必须说明的</t>
+  </si>
+  <si>
+    <t>stack</t>
+  </si>
+  <si>
+    <t>stack.pop()/stack.push() 返回/推入栈顶值</t>
+  </si>
+  <si>
+    <t>stack.pop2()/stack.push2() 返回/推入栈顶一个双字</t>
+  </si>
+  <si>
+    <t>stack.popf()/stack.pushf() 返回/推入栈顶一个float</t>
+  </si>
+  <si>
+    <t>调用一个方法，第一个参数为类名，第二个为方法名，第三个为存放参数的栈</t>
+  </si>
+  <si>
+    <t>jmp</t>
+  </si>
+  <si>
+    <t>以第一个参数为偏移量转到字节码区相应的位置（参数为u2）</t>
+  </si>
+  <si>
+    <t>ljmp</t>
+  </si>
+  <si>
+    <t>以第一个参数为偏移量转到字节码区相应的位置（参数为u4）</t>
   </si>
 </sst>
 </file>
@@ -799,10 +907,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1351,7 +1459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1360,10 +1468,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1372,7 +1480,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1496,7 +1604,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1552,7 +1660,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1563,23 +1671,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1900,10 +2017,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2070,10 +2187,10 @@
         <v>36</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>38</v>
@@ -2109,12 +2226,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" ht="28.5" spans="1:8">
+    <row r="12" spans="1:8">
       <c r="A12" s="12"/>
       <c r="B12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -2139,7 +2256,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" ht="28.5" spans="1:8">
       <c r="A14" s="12"/>
       <c r="B14" s="3" t="s">
         <v>55</v>
@@ -2154,290 +2271,292 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" ht="28.5" spans="1:8">
       <c r="A15" s="12"/>
       <c r="B15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="12"/>
       <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="G16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" ht="28.5" spans="1:8">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="12"/>
       <c r="B17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="G17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" ht="28.5" spans="1:8">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="12"/>
       <c r="B18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="G18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" ht="28.5" spans="1:8">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="G19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" ht="15" customHeight="1" spans="1:8">
+    </row>
+    <row r="20" ht="30" customHeight="1" spans="1:8">
       <c r="A20" s="15"/>
       <c r="B20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="G20" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+    </row>
+    <row r="21" ht="28.5" spans="1:8">
       <c r="A21" s="15"/>
       <c r="B21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="G21" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+    </row>
+    <row r="22" ht="28.5" spans="1:8">
       <c r="A22" s="15"/>
       <c r="B22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="G22" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+    </row>
+    <row r="23" ht="28.5" spans="1:8">
       <c r="A23" s="15"/>
       <c r="B23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="G23" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+    </row>
+    <row r="24" ht="28.5" spans="1:8">
       <c r="A24" s="15"/>
       <c r="B24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="G24" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="15"/>
       <c r="B25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="G25" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="15"/>
       <c r="B26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="G26" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="15"/>
       <c r="B27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="G27" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="15"/>
       <c r="B28" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="G28" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="15"/>
       <c r="B29" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="G29" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="15"/>
       <c r="B30" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="G30" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="31" ht="16" customHeight="1" spans="1:8">
       <c r="A31" s="16"/>
       <c r="B31" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="G31" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" spans="1:8">
       <c r="A32" s="16"/>
       <c r="B32" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="G32" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="16"/>
       <c r="B33" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="G33" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H33" s="17"/>
-    </row>
-    <row r="34" ht="28.5" spans="1:8">
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="16"/>
       <c r="B34" s="3" t="s">
         <v>134</v>
@@ -2452,7 +2571,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" ht="28.5" spans="1:8">
+    <row r="35" spans="1:8">
       <c r="A35" s="16"/>
       <c r="B35" s="3" t="s">
         <v>138</v>
@@ -2475,9 +2594,6 @@
       <c r="C36" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="G36" s="4" t="s">
         <v>144</v>
       </c>
@@ -2493,9 +2609,6 @@
       <c r="C37" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G37" s="4" t="s">
         <v>148</v>
       </c>
@@ -2511,152 +2624,131 @@
       <c r="C38" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="G38" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="39" ht="28.5" spans="1:8">
       <c r="A39" s="16"/>
       <c r="B39" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="G39" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G39" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="H39" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" ht="28.5" spans="1:8">
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="16"/>
       <c r="B40" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="G40" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="41" ht="28.5" spans="1:8">
       <c r="A41" s="16"/>
       <c r="B41" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="H41" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="42" ht="28.5" spans="1:8">
       <c r="A42" s="16"/>
       <c r="B42" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="G42" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G42" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="43" ht="28.5" spans="1:8">
       <c r="A43" s="16"/>
       <c r="B43" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="G43" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G43" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="44" ht="28.5" spans="1:8">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="16"/>
       <c r="B44" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G44" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H44" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="45" ht="28.5" spans="1:8">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="16"/>
       <c r="B45" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" s="4" t="s">
+      <c r="H45" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="H45" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" ht="28.5" spans="1:8">
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="16"/>
       <c r="B46" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>184</v>
@@ -2665,7 +2757,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" ht="28.5" spans="1:8">
       <c r="A47" s="16"/>
       <c r="B47" s="3" t="s">
         <v>186</v>
@@ -2673,6 +2765,9 @@
       <c r="C47" s="2" t="s">
         <v>187</v>
       </c>
+      <c r="D47" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="G47" s="4" t="s">
         <v>188</v>
       </c>
@@ -2680,7 +2775,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" ht="28.5" spans="1:8">
       <c r="A48" s="16"/>
       <c r="B48" s="3" t="s">
         <v>190</v>
@@ -2688,6 +2783,9 @@
       <c r="C48" s="2" t="s">
         <v>191</v>
       </c>
+      <c r="D48" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="G48" s="4" t="s">
         <v>192</v>
       </c>
@@ -2695,7 +2793,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" ht="28.5" spans="1:8">
       <c r="A49" s="16"/>
       <c r="B49" s="3" t="s">
         <v>194</v>
@@ -2703,192 +2801,189 @@
       <c r="C49" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="D49" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="G49" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H49" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="H49" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+    </row>
+    <row r="50" ht="28.5" spans="1:8">
       <c r="A50" s="16"/>
       <c r="B50" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="H50" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" ht="28.5" spans="2:8">
       <c r="B51" s="3" t="s">
         <v>201</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="D51" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="G51" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="52" spans="2:2">
+      <c r="H51" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" ht="28.5" spans="2:8">
       <c r="B52" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2">
+        <v>205</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="53" ht="28.5" spans="2:8">
       <c r="B53" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2">
+        <v>209</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" ht="28.5" spans="2:8">
       <c r="B54" s="3" t="s">
-        <v>206</v>
+        <v>213</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="3" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>209</v>
+        <v>218</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>219</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" ht="28.5" spans="2:8">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8">
       <c r="B56" s="3" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>32</v>
+        <v>222</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" ht="16" customHeight="1" spans="2:8">
       <c r="B57" s="3" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>32</v>
+        <v>226</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="58" ht="57" customHeight="1" spans="2:7">
       <c r="B58" s="3" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
       <c r="G58" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7">
       <c r="B59" s="3" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="D59" s="18"/>
       <c r="G59" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="60" ht="28.5" spans="2:8">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
       <c r="B60" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="61" ht="28.5" spans="2:9">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9">
       <c r="B61" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="I61" s="24"/>
-    </row>
-    <row r="62" ht="28.5" spans="1:9">
+        <v>237</v>
+      </c>
+      <c r="I61" s="23"/>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="19"/>
       <c r="B62" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="H62" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="I62" s="24"/>
+      <c r="I62" s="23"/>
     </row>
     <row r="63" ht="33" customHeight="1" spans="1:9">
       <c r="A63" s="20"/>
@@ -2901,90 +2996,303 @@
       <c r="D63" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="H63" s="22" t="s">
+      <c r="G63" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="I63" s="25"/>
+      <c r="H63" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I63" s="24"/>
     </row>
     <row r="64" ht="28.5" spans="1:9">
       <c r="A64" s="20"/>
       <c r="B64" s="21" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="E64" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G64" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="H64" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="I64" s="25"/>
-    </row>
-    <row r="65" ht="28.5" spans="2:9">
+      <c r="H64" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I64" s="24"/>
+    </row>
+    <row r="65" spans="2:9">
       <c r="B65" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C65" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="D65" s="21" t="s">
+      <c r="C65" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="H65" s="27" t="s">
+      <c r="G65" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="I65" s="24"/>
+      <c r="H65" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="I65" s="23"/>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C66" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="26" t="s">
+      <c r="C66" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="H66" s="27" t="s">
+      <c r="D66" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G66" s="4" t="s">
         <v>253</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="67" spans="2:8">
       <c r="B67" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="H67" s="22" t="s">
         <v>257</v>
       </c>
+      <c r="H67" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" ht="28.5" spans="3:8">
+      <c r="C68" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="69" ht="28.5" spans="3:8">
+      <c r="C69" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="70" ht="28.5" spans="3:8">
+      <c r="C70" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="71" ht="28.5" spans="3:8">
+      <c r="C71" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="72" ht="28.5" spans="3:8">
+      <c r="C72" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="H72" s="26" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="73" ht="28.5" spans="3:8">
+      <c r="C73" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="H73" s="28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8">
+      <c r="C74" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="H74" s="28" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8">
+      <c r="C75" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="H75" s="25" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8">
+      <c r="B78" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+    </row>
+    <row r="79" spans="3:8">
+      <c r="C79" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+    </row>
+    <row r="80" spans="3:8">
+      <c r="C80" s="10"/>
+      <c r="D80" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+    </row>
+    <row r="81" spans="3:8">
+      <c r="C81" s="10"/>
+      <c r="D81" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82" spans="3:8">
+      <c r="C82" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+    </row>
+    <row r="83" spans="3:8">
+      <c r="C83" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+    </row>
+    <row r="84" spans="3:8">
+      <c r="C84" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85" spans="3:8">
+      <c r="C85" s="29"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="30"/>
+      <c r="G85" s="30"/>
+      <c r="H85" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H32:H33"/>
+  <mergeCells count="10">
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="C78:H78"/>
+    <mergeCell ref="D79:H79"/>
+    <mergeCell ref="D80:H80"/>
+    <mergeCell ref="D81:H81"/>
+    <mergeCell ref="D82:H82"/>
+    <mergeCell ref="D83:H83"/>
+    <mergeCell ref="D84:H84"/>
+    <mergeCell ref="D85:H85"/>
+    <mergeCell ref="C79:C81"/>
   </mergeCells>
   <pageMargins left="0.118055555555556" right="0.118055555555556" top="0.156944444444444" bottom="0.118055555555556" header="0.3" footer="0.118055555555556"/>
   <pageSetup paperSize="9" orientation="landscape"/>

</xml_diff>